<commit_message>
[TASK] Update dossier, timesheet & presentation
</commit_message>
<xml_diff>
--- a/docs/timesheet_ilona_zancaner.xlsx
+++ b/docs/timesheet_ilona_zancaner.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
   <si>
     <t>Student</t>
   </si>
@@ -75,6 +75,171 @@
   </si>
   <si>
     <t>Design: wireframes website</t>
+  </si>
+  <si>
+    <t>Installeren van Drupal, modules &amp; vue project</t>
+  </si>
+  <si>
+    <t>Aanmaken van custom content types</t>
+  </si>
+  <si>
+    <t>Aanmaken van pages</t>
+  </si>
+  <si>
+    <t>Custom theme configuratie</t>
+  </si>
+  <si>
+    <t>Home page twig &amp; css</t>
+  </si>
+  <si>
+    <t>Contact page twig &amp; css</t>
+  </si>
+  <si>
+    <t>Features page twig &amp; css</t>
+  </si>
+  <si>
+    <t>Features content type configureren</t>
+  </si>
+  <si>
+    <t>Vehicles inladen in vue frontend</t>
+  </si>
+  <si>
+    <t>Vehicle detail page</t>
+  </si>
+  <si>
+    <t>Feature - Nieuw Vehicle aanmaken</t>
+  </si>
+  <si>
+    <t>Vehicle omzetten in Entity</t>
+  </si>
+  <si>
+    <t>Productiedossier deployment guide</t>
+  </si>
+  <si>
+    <t>Productiedossier handleiding</t>
+  </si>
+  <si>
+    <t>Productiedossier layout aanpassen</t>
+  </si>
+  <si>
+    <t>Productiedossier style guide</t>
+  </si>
+  <si>
+    <t>Productiedossier planning aanpassen</t>
+  </si>
+  <si>
+    <t>Fix CORS error</t>
+  </si>
+  <si>
+    <t>Overview page css</t>
+  </si>
+  <si>
+    <t>Detail page css</t>
+  </si>
+  <si>
+    <t>Update voor Vehicle Entity</t>
+  </si>
+  <si>
+    <t>Registreren van nieuwe user</t>
+  </si>
+  <si>
+    <t>Login voor bestaande users</t>
+  </si>
+  <si>
+    <t>Profiel page css</t>
+  </si>
+  <si>
+    <t>Bug fix broken/missing handler</t>
+  </si>
+  <si>
+    <t>Voertuigen inladen van bestaande user</t>
+  </si>
+  <si>
+    <t>Aanmaken van voertuig door ingelogde user</t>
+  </si>
+  <si>
+    <t>Voertuig kunnen huren</t>
+  </si>
+  <si>
+    <t>Responsive maken van profiel page</t>
+  </si>
+  <si>
+    <t>Reponsive maken van overview page</t>
+  </si>
+  <si>
+    <t>Responsive maken van detail page</t>
+  </si>
+  <si>
+    <t>Velden van Vehicle entity aanpassen</t>
+  </si>
+  <si>
+    <t>Review entity aanmaken</t>
+  </si>
+  <si>
+    <t>Velden van Review entity aanpassen</t>
+  </si>
+  <si>
+    <t>Homepage component</t>
+  </si>
+  <si>
+    <t>Rental entity aanmaken</t>
+  </si>
+  <si>
+    <t>Reviews tonen in detail page</t>
+  </si>
+  <si>
+    <t>Nieuw review aanmaken</t>
+  </si>
+  <si>
+    <t>Vehicle entity updaten</t>
+  </si>
+  <si>
+    <t>"Create Vehicle" verder uitbreiden</t>
+  </si>
+  <si>
+    <t>Rental entity updaten</t>
+  </si>
+  <si>
+    <t>Rentals tonen</t>
+  </si>
+  <si>
+    <t>Rental verwijderen</t>
+  </si>
+  <si>
+    <t>Fix bug registered user werd niet ingelogd</t>
+  </si>
+  <si>
+    <t>Wachtwoord opslaan in local storage</t>
+  </si>
+  <si>
+    <t>Code detail page opruimen</t>
+  </si>
+  <si>
+    <t>Image field voorzien voor Vehicle</t>
+  </si>
+  <si>
+    <t>Drupal website aanpassen</t>
+  </si>
+  <si>
+    <t>Drupal website home responsive maken</t>
+  </si>
+  <si>
+    <t>Fix bug met reviews die niet laden</t>
+  </si>
+  <si>
+    <t>Fix fouten namen in API</t>
+  </si>
+  <si>
+    <t>Fix update vehicle wou type niet updaten</t>
+  </si>
+  <si>
+    <t>Detail page css aanpassen</t>
+  </si>
+  <si>
+    <t>Dossier aanpassen</t>
+  </si>
+  <si>
+    <t>Presentatie</t>
   </si>
 </sst>
 </file>
@@ -179,7 +344,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -190,15 +355,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -488,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H128"/>
+  <dimension ref="A1:H108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -503,27 +664,27 @@
     <col min="7" max="8" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15"/>
-    </row>
-    <row r="2" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43049</v>
       </c>
@@ -534,7 +695,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43049</v>
       </c>
@@ -545,7 +706,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43052</v>
       </c>
@@ -556,7 +717,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43052</v>
       </c>
@@ -568,9 +729,9 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>43053</v>
+        <v>43052</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -579,9 +740,9 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>43053</v>
+        <v>43052</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -590,9 +751,9 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>43053</v>
+        <v>43052</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -601,9 +762,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43053</v>
+        <v>43052</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -612,9 +773,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>43053</v>
+        <v>43052</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -623,9 +784,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>43053</v>
+        <v>43052</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
@@ -634,54 +795,711 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="4">
-        <f>SUM(C3:C12)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-    </row>
-    <row r="29" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-    </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>43053</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>43053</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43053</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>43053</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>43059</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="3">
+        <f>0.5+0.75+0.5</f>
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>43060</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43062</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>43063</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43066</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>43066</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>43092</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>43107</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="3">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>43107</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="3">
+        <f>0.25+1.25+0.5</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>43108</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>43108</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="3">
+        <f>1.25+0.25+0.75+0.25</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>43108</v>
+      </c>
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="3">
+        <f>1+0.5+0.5+0.5</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>43108</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>43108</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>43108</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>43108</v>
+      </c>
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>43108</v>
+      </c>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="3">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>43114</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="3">
+        <f>0.25+0.75+0.5</f>
+        <v>1.5</v>
+      </c>
       <c r="G36" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D91" s="13"/>
-      <c r="E91" s="13"/>
-    </row>
-    <row r="92" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D92" s="14"/>
-      <c r="E92" s="14"/>
-      <c r="F92" s="12"/>
-      <c r="G92" s="11"/>
-    </row>
-    <row r="127" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E127" s="10"/>
-      <c r="F127" s="10"/>
-      <c r="G127" s="10"/>
-    </row>
-    <row r="128" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E128" s="11"/>
-      <c r="F128" s="11"/>
-      <c r="G128" s="11"/>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>43114</v>
+      </c>
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>43114</v>
+      </c>
+      <c r="B38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>43114</v>
+      </c>
+      <c r="B39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>43114</v>
+      </c>
+      <c r="B40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>43114</v>
+      </c>
+      <c r="B41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>43114</v>
+      </c>
+      <c r="B42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" s="3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>43114</v>
+      </c>
+      <c r="B43" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>43115</v>
+      </c>
+      <c r="B44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>43115</v>
+      </c>
+      <c r="B45" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" s="3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>43115</v>
+      </c>
+      <c r="B46" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>43115</v>
+      </c>
+      <c r="B47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47" s="3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>43115</v>
+      </c>
+      <c r="B48" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>43115</v>
+      </c>
+      <c r="B49" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>43115</v>
+      </c>
+      <c r="B50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>43115</v>
+      </c>
+      <c r="B51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>43115</v>
+      </c>
+      <c r="B52" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>43116</v>
+      </c>
+      <c r="B53" t="s">
+        <v>51</v>
+      </c>
+      <c r="C53" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>43116</v>
+      </c>
+      <c r="B54" t="s">
+        <v>52</v>
+      </c>
+      <c r="C54" s="3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>43116</v>
+      </c>
+      <c r="B55" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55" s="3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>43116</v>
+      </c>
+      <c r="B56" t="s">
+        <v>54</v>
+      </c>
+      <c r="C56" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>43116</v>
+      </c>
+      <c r="B57" t="s">
+        <v>55</v>
+      </c>
+      <c r="C57" s="3">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>43116</v>
+      </c>
+      <c r="B58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C58" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>43116</v>
+      </c>
+      <c r="B59" t="s">
+        <v>57</v>
+      </c>
+      <c r="C59" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>43116</v>
+      </c>
+      <c r="B60" t="s">
+        <v>58</v>
+      </c>
+      <c r="C60" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>43116</v>
+      </c>
+      <c r="B61" t="s">
+        <v>59</v>
+      </c>
+      <c r="C61" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>43116</v>
+      </c>
+      <c r="B62" t="s">
+        <v>60</v>
+      </c>
+      <c r="C62" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>43116</v>
+      </c>
+      <c r="B63" t="s">
+        <v>61</v>
+      </c>
+      <c r="C63" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>43116</v>
+      </c>
+      <c r="B64" t="s">
+        <v>62</v>
+      </c>
+      <c r="C64" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>43116</v>
+      </c>
+      <c r="B65" t="s">
+        <v>63</v>
+      </c>
+      <c r="C65" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>43116</v>
+      </c>
+      <c r="B66" t="s">
+        <v>64</v>
+      </c>
+      <c r="C66" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>43116</v>
+      </c>
+      <c r="B67" t="s">
+        <v>65</v>
+      </c>
+      <c r="C67" s="3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>43116</v>
+      </c>
+      <c r="B68" t="s">
+        <v>66</v>
+      </c>
+      <c r="C68" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>43116</v>
+      </c>
+      <c r="B69" t="s">
+        <v>67</v>
+      </c>
+      <c r="C69" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>43116</v>
+      </c>
+      <c r="B70" t="s">
+        <v>68</v>
+      </c>
+      <c r="C70" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>43116</v>
+      </c>
+      <c r="B71" t="s">
+        <v>69</v>
+      </c>
+      <c r="C71" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>43117</v>
+      </c>
+      <c r="B72" t="s">
+        <v>70</v>
+      </c>
+      <c r="C72" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>43117</v>
+      </c>
+      <c r="B73" t="s">
+        <v>71</v>
+      </c>
+      <c r="C73" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="5"/>
+      <c r="B74" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="4">
+        <f>SUM(C3:C73)</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E107" s="9"/>
+      <c r="F107" s="9"/>
+      <c r="G107" s="9"/>
+    </row>
+    <row r="108" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E108" s="10"/>
+      <c r="F108" s="10"/>
+      <c r="G108" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>